<commit_message>
[RPG] Multidoodads (rock, tree)
- Rajouté la gestion de plusieurs doodads (tree et rock).
- Changé comment l'affichage des doodads est géré.
- Réorganiser les ressources graphiques.
- Relié main.py et matrix_map.py
- Couche sol
- Couche doodad
</commit_message>
<xml_diff>
--- a/assets/map/map01.xlsx
+++ b/assets/map/map01.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tallentaa\assets\map\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28680" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ground" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>water</t>
   </si>
@@ -30,22 +35,16 @@
     <t>grass</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Tree</t>
   </si>
   <si>
     <t>BigRock</t>
   </si>
-  <si>
-    <t>R</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,6 +199,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -247,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,9 +282,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,6 +334,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,11 +526,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN4" sqref="AN4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3648,11 +3684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3672,7 +3708,9 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="L1" s="7">
+        <v>9</v>
+      </c>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="10"/>
@@ -3790,8 +3828,8 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10" t="s">
-        <v>4</v>
+      <c r="S4" s="10">
+        <v>5</v>
       </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -3909,8 +3947,8 @@
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
-      <c r="Y7" s="10" t="s">
-        <v>4</v>
+      <c r="Y7" s="10">
+        <v>5</v>
       </c>
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
@@ -3947,8 +3985,8 @@
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
-      <c r="X8" s="10" t="s">
-        <v>4</v>
+      <c r="X8" s="10">
+        <v>5</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
@@ -4103,8 +4141,8 @@
       <c r="AA12" s="10"/>
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
-      <c r="AD12" s="10" t="s">
-        <v>4</v>
+      <c r="AD12" s="10">
+        <v>5</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="10"/>
@@ -4326,7 +4364,9 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
+      <c r="AC18" s="7">
+        <v>9</v>
+      </c>
       <c r="AD18" s="7"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="10"/>
@@ -4448,8 +4488,8 @@
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
-        <v>4</v>
+      <c r="C22" s="10">
+        <v>5</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4714,8 +4754,8 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="10" t="s">
-        <v>4</v>
+      <c r="H29" s="10">
+        <v>5</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -4731,7 +4771,9 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
+      <c r="W29" s="7">
+        <v>9</v>
+      </c>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
@@ -4747,8 +4789,8 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
-      <c r="B30" s="10" t="s">
-        <v>4</v>
+      <c r="B30" s="10">
+        <v>5</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -4965,11 +5007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5022,19 +5064,19 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>